<commit_message>
Fixed active cell in test files
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/borders_with_hidden_rows_and_columns.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/borders_with_hidden_rows_and_columns.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svn\GIT\tagetik-2017-spreadsheet-1.4\tagetik-2017-spreadsheet\vaadin-spreadsheet\src\test\resources\test_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Borders" sheetId="1" r:id="rId1"/>
     <sheet name="Merged cells" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -125,6 +125,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -134,16 +135,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Norm." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -418,37 +421,37 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="7.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="7.375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="16" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I10" s="2"/>
     </row>
   </sheetData>
@@ -460,65 +463,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="8" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="10.875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:11" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:11" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="9"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+    <row r="5" spans="1:11" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="10"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
+    <row r="9" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H11" s="6"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G12" s="7"/>
-      <c r="H12" s="8"/>
+    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="2"/>
       <c r="J12" s="5"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H13" s="3"/>
       <c r="J13" s="3"/>
     </row>

</xml_diff>